<commit_message>
Azurirala slucajeve upotrebe i dodala novi
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/IzdavanjePotvrdeONekaznjavanju.xlsx
+++ b/UseCaseIScenarij/IzdavanjePotvrdeONekaznjavanju.xlsx
@@ -284,12 +284,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -328,16 +340,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -656,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,24 +724,24 @@
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -738,7 +751,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -748,22 +761,22 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>